<commit_message>
add next match column to scrape_bracket to simplify prediction tool
</commit_message>
<xml_diff>
--- a/bracket.xlsx
+++ b/bracket.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="153">
   <si>
     <t>Index</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Round</t>
   </si>
   <si>
+    <t>Next Match</t>
+  </si>
+  <si>
     <t>01</t>
   </si>
   <si>
@@ -457,7 +460,10 @@
     <t>SOUTH</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Final Four</t>
+  </si>
+  <si>
+    <t>Championship</t>
   </si>
   <si>
     <t>WEST</t>
@@ -466,25 +472,7 @@
     <t>MIDWEST</t>
   </si>
   <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>sweet 16</t>
-  </si>
-  <si>
-    <t>elite 8</t>
-  </si>
-  <si>
-    <t>final 4</t>
-  </si>
-  <si>
-    <t>championship</t>
-  </si>
-  <si>
-    <t>first 4</t>
+    <t>First Four</t>
   </si>
 </sst>
 </file>
@@ -842,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,1948 +864,2152 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
       <c r="H4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
-        <v>145</v>
-      </c>
-      <c r="I11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>145</v>
-      </c>
-      <c r="I13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H14" t="s">
-        <v>145</v>
-      </c>
-      <c r="I14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
-      </c>
-      <c r="I15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H16" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>146</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H17" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>146</v>
-      </c>
-      <c r="I19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H20" t="s">
-        <v>146</v>
-      </c>
-      <c r="I20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
-        <v>146</v>
-      </c>
-      <c r="I21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>146</v>
-      </c>
-      <c r="I24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H25" t="s">
-        <v>146</v>
-      </c>
-      <c r="I25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H26" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H27" t="s">
-        <v>146</v>
-      </c>
-      <c r="I27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>146</v>
-      </c>
-      <c r="I28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
         <v>30</v>
       </c>
-      <c r="D29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>138</v>
-      </c>
-      <c r="H29" t="s">
-        <v>146</v>
-      </c>
-      <c r="I29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="C30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" t="s">
-        <v>16</v>
-      </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H30" t="s">
-        <v>146</v>
-      </c>
-      <c r="I30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>147</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
         <v>33</v>
       </c>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" t="s">
-        <v>65</v>
-      </c>
-      <c r="H31" t="s">
-        <v>146</v>
-      </c>
-      <c r="I31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H32" t="s">
-        <v>147</v>
-      </c>
-      <c r="I32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>148</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H33" t="s">
-        <v>147</v>
-      </c>
-      <c r="I33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>149</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>148</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G35" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H35" t="s">
-        <v>148</v>
-      </c>
-      <c r="I35" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" t="s">
+        <v>150</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
         <v>42</v>
       </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" t="s">
-        <v>148</v>
-      </c>
-      <c r="I36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" t="s">
+        <v>150</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
         <v>43</v>
       </c>
-      <c r="D37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37" t="s">
-        <v>148</v>
-      </c>
-      <c r="I37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G38" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H38" t="s">
-        <v>148</v>
-      </c>
-      <c r="I38" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H39" t="s">
-        <v>148</v>
-      </c>
-      <c r="I39" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H40" t="s">
-        <v>148</v>
-      </c>
-      <c r="I40" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H41" t="s">
-        <v>148</v>
-      </c>
-      <c r="I41" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H42" t="s">
-        <v>148</v>
-      </c>
-      <c r="I42" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H43" t="s">
-        <v>148</v>
-      </c>
-      <c r="I43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G44" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H44" t="s">
-        <v>148</v>
-      </c>
-      <c r="I44" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H45" t="s">
-        <v>148</v>
-      </c>
-      <c r="I45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H46" t="s">
+        <v>150</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
         <v>47</v>
       </c>
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E46" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" t="s">
-        <v>90</v>
-      </c>
-      <c r="H46" t="s">
-        <v>148</v>
-      </c>
-      <c r="I46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H47" t="s">
-        <v>148</v>
-      </c>
-      <c r="I47" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" t="s">
         <v>74</v>
       </c>
-      <c r="E48" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="H48" t="s">
+        <v>150</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
         <v>48</v>
       </c>
-      <c r="G48" t="s">
-        <v>73</v>
-      </c>
-      <c r="H48" t="s">
-        <v>148</v>
-      </c>
-      <c r="I48" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H49" t="s">
-        <v>148</v>
-      </c>
-      <c r="I49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="J49">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E50" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G50" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H50" t="s">
-        <v>149</v>
-      </c>
-      <c r="I50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E51" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H51" t="s">
-        <v>149</v>
-      </c>
-      <c r="I51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E52" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H52" t="s">
-        <v>149</v>
-      </c>
-      <c r="I52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F53" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G53" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H53" t="s">
-        <v>149</v>
-      </c>
-      <c r="I53" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F54" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G54" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H54" t="s">
-        <v>149</v>
-      </c>
-      <c r="I54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H55" t="s">
-        <v>149</v>
-      </c>
-      <c r="I55" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D56" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F56" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" t="s">
+        <v>142</v>
+      </c>
+      <c r="H56" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
         <v>60</v>
       </c>
-      <c r="G56" t="s">
-        <v>141</v>
-      </c>
-      <c r="H56" t="s">
-        <v>149</v>
-      </c>
-      <c r="I56" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E57" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F57" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H57" t="s">
-        <v>149</v>
-      </c>
-      <c r="I57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D58" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G58" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H58" t="s">
-        <v>149</v>
-      </c>
-      <c r="I58" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G59" t="s">
         <v>89</v>
       </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>53</v>
-      </c>
-      <c r="G59" t="s">
-        <v>88</v>
-      </c>
       <c r="H59" t="s">
-        <v>149</v>
-      </c>
-      <c r="I59" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G60" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H60" t="s">
-        <v>149</v>
-      </c>
-      <c r="I60" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G61" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H61" t="s">
-        <v>149</v>
-      </c>
-      <c r="I61" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="I61">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G62" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H62" t="s">
-        <v>149</v>
-      </c>
-      <c r="I62" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+      <c r="J62">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" t="s">
         <v>70</v>
       </c>
-      <c r="E63" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" t="s">
-        <v>57</v>
-      </c>
-      <c r="G63" t="s">
-        <v>69</v>
-      </c>
       <c r="H63" t="s">
-        <v>149</v>
-      </c>
-      <c r="I63" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I63">
+        <v>3</v>
+      </c>
+      <c r="J63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G64" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H64" t="s">
-        <v>149</v>
-      </c>
-      <c r="I64" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>151</v>
+      </c>
+      <c r="I64">
+        <v>4</v>
+      </c>
+      <c r="J64">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D65" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G65" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H65" t="s">
-        <v>147</v>
-      </c>
-      <c r="I65" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>152</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E66" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H66" t="s">
-        <v>147</v>
-      </c>
-      <c r="I66" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>152</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E67" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F67" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G67" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H67" t="s">
-        <v>147</v>
-      </c>
-      <c r="I67" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>152</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G68" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H68" t="s">
-        <v>147</v>
-      </c>
-      <c r="I68" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>